<commit_message>
add pagintion,spring mvc,web.xml 404,500error page
</commit_message>
<xml_diff>
--- a/test/develop/develop.xlsx
+++ b/test/develop/develop.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2775" windowWidth="18825" windowHeight="5010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2775" windowWidth="13005" windowHeight="4440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="问题列表" sheetId="1" r:id="rId1"/>
     <sheet name="提交日志" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1:C7"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>问题名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -79,6 +80,30 @@
   </si>
   <si>
     <t>提交的HashCode值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6ebd276f07d83a7c4cddd2bd8cbe2dd62024bc9e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>何超杰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>问题1：SpringMVC Controller是单例模式，尽量避免在Controller类中声明成员变量，以免多线程共享数据，导致数据不安全情况。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>问题2：自己写简单的分页器Pagination，在Controller设置分页的PathURL。暂未对分页插件进行CSS优化，后续处理。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>问题3：Spring设置prefix：前缀, suffix：后缀，在Controller方便可省略跳转的jsp后缀及前缀。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>问题4：在Servlet中转发首页，配置404，500错误并指向首页。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -149,7 +174,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -179,9 +204,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -483,7 +505,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -656,13 +678,13 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="14.125" customWidth="1"/>
-    <col min="2" max="2" width="12.25" customWidth="1"/>
+    <col min="1" max="1" width="14.125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="7" customWidth="1"/>
     <col min="3" max="3" width="54.25" style="4" customWidth="1"/>
     <col min="4" max="4" width="43.25" style="7" customWidth="1"/>
   </cols>
@@ -674,7 +696,7 @@
       <c r="B1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="6" t="s">
@@ -691,7 +713,9 @@
       <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="40.5">
       <c r="A3" s="6"/>
@@ -701,75 +725,87 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="2"/>
+    <row r="4" spans="1:4" ht="40.5">
+      <c r="A4" s="8">
+        <v>41979</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="2"/>
+    <row r="5" spans="1:4" ht="27">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="2"/>
+    <row r="6" spans="1:4" ht="27">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="2"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="2"/>
       <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="2"/>
       <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="2"/>
       <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
       <c r="C11" s="2"/>
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="2"/>
       <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
       <c r="C13" s="2"/>
       <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
       <c r="C14" s="2"/>
       <c r="D14" s="6"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
       <c r="C15" s="2"/>
       <c r="D15" s="6"/>
     </row>

</xml_diff>

<commit_message>
add solr4.5 and mmseg4j1.9
</commit_message>
<xml_diff>
--- a/test/develop/develop.xlsx
+++ b/test/develop/develop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2775" windowWidth="17745" windowHeight="5130" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2775" windowWidth="13695" windowHeight="2940" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="问题列表" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
   <si>
     <t>问题名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -193,6 +193,14 @@
   </si>
   <si>
     <t>问题3:增加定时任务配置表,可控制定时任务启动停止。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>问题1:更新solr3.5到solr4.5支持。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>问题2:更新mmseg4j1.8到mmseg4j1.9支持。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -838,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1011,15 +1019,23 @@
       <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="2"/>
+      <c r="A16" s="8">
+        <v>41984</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="D16" s="6"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="D17" s="6"/>
     </row>
     <row r="18" spans="1:4">

</xml_diff>